<commit_message>
Alt3 with no regex
</commit_message>
<xml_diff>
--- a/CH-169 Extract From Text Part 2.xlsx
+++ b/CH-169 Extract From Text Part 2.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B794D0A6-9C13-44D7-B6B7-AAEE22CED814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEF3160-AB07-4C1F-BBB0-E5177D74BB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
     <sheet name="Alt2" sheetId="4" r:id="rId4"/>
+    <sheet name="Alt3" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$C$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$B$2:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Alt3'!$B$2:$C$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$C$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$C$13</definedName>
   </definedNames>
@@ -92,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="17">
   <si>
     <t>Question</t>
   </si>
@@ -490,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -531,6 +533,12 @@
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1020,6 +1028,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="401" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{BAD9B4BC-CD4A-4EC5-AAEF-10E05DC3E3A8}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
@@ -1340,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469A7F93-5D73-45B6-BB59-575C06EC4AA0}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1632,4 +1667,230 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B280B5E-DF09-4007-BA6E-D550570EFCEB}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="52.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.3984375" customWidth="1"/>
+    <col min="4" max="4" width="24.69921875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="19" t="str" cm="1">
+        <f t="array" ref="D10:D14">_xlfn.MAP(
+    B3:B7,
+    _xlfn.LAMBDA(_xlpm.x,
+        _xlfn.TEXTJOIN(
+            ", ",
+            ,
+            INDEX(
+                _xlfn.TEXTSPLIT(
+                    _xlpm.x,
+                    {"{","[","*","("},
+                    {"}","]","*",")"},
+                    1,
+                    ,
+                ),
+                ,
+                2
+            )
+        )
+    )
+)</f>
+        <v>quick brown</v>
+      </c>
+      <c r="F10" t="str" cm="1">
+        <f t="array" ref="F10:G11">_xlfn.TEXTSPLIT(
+                    B3,
+                    {"{","[","*","("},
+                    {"}","]","*",")"},
+                    1,
+                    ,
+                )</f>
+        <v xml:space="preserve">The </v>
+      </c>
+      <c r="G10" t="str">
+        <v>quick brown</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="str" cm="1">
+        <f t="array" ref="B11:B15">_xlfn.MAP(
+    B3:B7,
+    _xlfn.LAMBDA(_xlpm.x,
+        _xlfn.TEXTJOIN(
+            ", ",
+            ,
+            INDEX(
+                _xlfn.TEXTSPLIT(
+                    _xlpm.x,
+                    {"{","[","*","("},
+                    {"}","]","*",")"},
+                    1,
+                    ,
+                ),
+                ,
+                2
+            )
+        )
+    )
+)</f>
+        <v>quick brown</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="20" t="str">
+        <v>reading books, Walking</v>
+      </c>
+      <c r="F11" t="str">
+        <v xml:space="preserve"> fox jumps over the lazy dog.</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="str">
+        <v>reading books, Walking</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="19" t="str">
+        <v>beach for, fun</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="str">
+        <v>beach for, fun</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="19" t="str">
+        <v>chocolate cake, delicious, rich</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="str">
+        <v>chocolate cake, delicious, rich</v>
+      </c>
+      <c r="D14" s="19" t="str">
+        <v>playing guitar</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="str">
+        <v>playing guitar</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on my breakdown
</commit_message>
<xml_diff>
--- a/CH-169 Extract From Text Part 2.xlsx
+++ b/CH-169 Extract From Text Part 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEF3160-AB07-4C1F-BBB0-E5177D74BB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BE9222-1A0F-4E48-8ADA-B02543F8D89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,7 +346,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -365,6 +365,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -492,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -540,6 +552,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,7 +1044,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="401" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="471" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1042,7 +1056,9 @@
   <we:alternateReferences>
     <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
   </we:alternateReferences>
-  <we:properties/>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{10692169-43F9-4000-86B7-0A57F5434878}&quot;}"/>
+  </we:properties>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
@@ -1671,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B280B5E-DF09-4007-BA6E-D550570EFCEB}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="H14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1684,9 +1700,10 @@
     <col min="3" max="3" width="4.3984375" customWidth="1"/>
     <col min="4" max="4" width="24.69921875" style="5" customWidth="1"/>
     <col min="7" max="7" width="11.796875" customWidth="1"/>
+    <col min="8" max="8" width="51.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1697,7 +1714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>6</v>
       </c>
@@ -1706,7 +1723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>2</v>
       </c>
@@ -1720,7 +1737,7 @@
       <c r="H3" s="8"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1734,7 +1751,7 @@
       <c r="H4" s="8"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>9</v>
       </c>
@@ -1748,7 +1765,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>13</v>
       </c>
@@ -1762,7 +1779,7 @@
       <c r="H6" s="8"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
@@ -1771,18 +1788,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8" s="22" t="str">
+        <f>B4</f>
+        <v>She enjoys [reading books] and [Walking] on rainy days.</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1809,21 +1830,30 @@
 )</f>
         <v>quick brown</v>
       </c>
-      <c r="F10" t="str" cm="1">
-        <f t="array" ref="F10:G11">_xlfn.TEXTSPLIT(
-                    B3,
+      <c r="H10" t="str" cm="1">
+        <f t="array" ref="H10:I12">_xlfn.TEXTSPLIT(
+                    H8,
                     {"{","[","*","("},
                     {"}","]","*",")"},
-                    1,
+                    TRUE,
                     ,
+""
                 )</f>
-        <v xml:space="preserve">The </v>
-      </c>
-      <c r="G10" t="str">
-        <v>quick brown</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">She enjoys </v>
+      </c>
+      <c r="I10" t="str">
+        <v>reading books</v>
+      </c>
+      <c r="L10" t="str" cm="1">
+        <f t="array" ref="L10:L12">INDEX(_xlfn.ANCHORARRAY(H10), , 2)</f>
+        <v>reading books</v>
+      </c>
+      <c r="O10" s="21" t="str">
+        <f>_xlfn.TEXTJOIN(",",,_xlfn.ANCHORARRAY(L10))</f>
+        <v>reading books,Walking</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str" cm="1">
         <f t="array" ref="B11:B15">_xlfn.MAP(
     B3:B7,
@@ -1851,14 +1881,17 @@
       <c r="D11" s="20" t="str">
         <v>reading books, Walking</v>
       </c>
-      <c r="F11" t="str">
-        <v xml:space="preserve"> fox jumps over the lazy dog.</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" t="str">
+        <v xml:space="preserve"> and </v>
+      </c>
+      <c r="I11" t="str">
+        <v>Walking</v>
+      </c>
+      <c r="L11" t="str">
+        <v>Walking</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="str">
         <v>reading books, Walking</v>
       </c>
@@ -1866,8 +1899,17 @@
       <c r="D12" s="19" t="str">
         <v>beach for, fun</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" t="str">
+        <v xml:space="preserve"> on rainy days.</v>
+      </c>
+      <c r="I12" t="str">
+        <v/>
+      </c>
+      <c r="L12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="str">
         <v>beach for, fun</v>
       </c>
@@ -1876,16 +1918,60 @@
         <v>chocolate cake, delicious, rich</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <v>chocolate cake, delicious, rich</v>
       </c>
       <c r="D14" s="19" t="str">
         <v>playing guitar</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14" t="str">
+        <f>O10</f>
+        <v>reading books,Walking</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
+        <v>playing guitar</v>
+      </c>
+      <c r="H15" t="str" cm="1">
+        <f t="array" ref="H15:H19">B3:B7</f>
+        <v>The (quick brown) fox jumps over the lazy dog.</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="dataTable" ref="I15:I19" dt2D="0" dtr="0" r1="H8"/>
+        <v>quick brown</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H16" t="str">
+        <v>She enjoys [reading books] and [Walking] on rainy days.</v>
+      </c>
+      <c r="I16" t="str">
+        <v>reading books,Walking</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17" t="str">
+        <v>They went to the {beach for} a *fun* weekend.</v>
+      </c>
+      <c r="I17" t="str">
+        <v>beach for,fun</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18" t="str">
+        <v>The (chocolate cake) was (delicious) and {rich}.</v>
+      </c>
+      <c r="I18" t="str">
+        <v>chocolate cake,delicious,rich</v>
+      </c>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19" t="str">
+        <v>He loves [playing guitar] in his free time.</v>
+      </c>
+      <c r="I19" t="str">
         <v>playing guitar</v>
       </c>
     </row>
@@ -1893,4 +1979,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10692169-43F9-4000-86B7-0A57F5434878}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Starting to breakdown regex
</commit_message>
<xml_diff>
--- a/CH-169 Extract From Text Part 2.xlsx
+++ b/CH-169 Extract From Text Part 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BE9222-1A0F-4E48-8ADA-B02543F8D89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF52680A-E31E-4F38-B2E0-3573F000CA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="23">
   <si>
     <t>Question</t>
   </si>
@@ -252,12 +252,107 @@
   <si>
     <t>Missing answers, Walking, fun</t>
   </si>
+  <si>
+    <t>".*?(\(([^\[{(*\]})]*)\)|\[((?2))]|{((?2))}|\*((?2))\*).*?(?=(?1)|($))</t>
+  </si>
+  <si>
+    <t>\[((?2))]</t>
+  </si>
+  <si>
+    <t>{((?2))}</t>
+  </si>
+  <si>
+    <t>\*((?2))\*).*?(?=(?1)</t>
+  </si>
+  <si>
+    <t>($))</t>
+  </si>
+  <si>
+    <r>
+      <t>".*?</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="0.39997558519241921"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[^\[{(*\]})]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="0.39997558519241921"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +440,30 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -504,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -554,6 +673,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,7 +1166,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="471" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1215,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B171B0C-5D2A-4231-8B3D-1BA0BFDBF0CC}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1389,10 +1511,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469A7F93-5D73-45B6-BB59-575C06EC4AA0}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1528,6 +1650,36 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="str">
         <v>playing guitar</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1689,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B280B5E-DF09-4007-BA6E-D550570EFCEB}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="E2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Trying to breakdown the Regex more
</commit_message>
<xml_diff>
--- a/CH-169 Extract From Text Part 2.xlsx
+++ b/CH-169 Extract From Text Part 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF52680A-E31E-4F38-B2E0-3573F000CA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7557770D-0B60-4BE9-8D62-448AD1C808FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
   <si>
     <t>Question</t>
   </si>
@@ -346,6 +346,9 @@
       </rPr>
       <t>\)</t>
     </r>
+  </si>
+  <si>
+    <t>beach for</t>
   </si>
 </sst>
 </file>
@@ -1184,6 +1187,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1337,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B171B0C-5D2A-4231-8B3D-1BA0BFDBF0CC}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1461,43 +1467,60 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="e" cm="1" vm="1">
-        <f t="array" ref="B12">_xlfn.REGEXEXTRACT(B3,"\{(.+?)\}|\*(.+?)\*",2)</f>
+        <f t="array" ref="B12">_xlfn.REGEXEXTRACT(B3,"(\{(.+?)\})|(\*(.+?)\*)",2)</f>
         <v>#N/A</v>
       </c>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="e" cm="1" vm="1">
-        <f t="array" ref="B13">_xlfn.REGEXEXTRACT(B4,"\{(.+?)\}|\*(.+?)\*",2)</f>
+        <f t="array" ref="B13">_xlfn.REGEXEXTRACT(B4,"(\{(.+?)\})|(\*(.+?)\*)",2)</f>
         <v>#N/A</v>
       </c>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str" cm="1">
-        <f t="array" ref="B14:C14">_xlfn.REGEXEXTRACT(B5,"\{(.+?)\}|\*(.+?)\*",2)</f>
+        <f t="array" ref="B14:E14">_xlfn.REGEXEXTRACT(B5,"(\{(.+?)\})|(\*(.+?)\*)",2)</f>
+        <v>{beach for}</v>
+      </c>
+      <c r="C14" t="str">
         <v>beach for</v>
       </c>
-      <c r="C14" t="e" vm="2">
+      <c r="D14" s="5" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="E14" t="e" vm="2">
         <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str" cm="1">
-        <f t="array" ref="B15:C15">_xlfn.REGEXEXTRACT(B6,"\{(.+?)\}|\*(.+?)\*",2)</f>
+        <f t="array" ref="B15:E15">_xlfn.REGEXEXTRACT(B6,"(\{(.+?)\})|(\*(.+?)\*)",2)</f>
+        <v>{rich}</v>
+      </c>
+      <c r="C15" t="str">
         <v>rich</v>
       </c>
-      <c r="C15" t="e" vm="2">
+      <c r="D15" s="5" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="E15" t="e" vm="2">
         <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="e" cm="1" vm="1">
-        <f t="array" ref="B16">_xlfn.REGEXEXTRACT(B7,"\{(.+?)\}|\*(.+?)\*",2)</f>
+        <f t="array" ref="B16">_xlfn.REGEXEXTRACT(B7,"(\{(.+?)\})|(\*(.+?)\*)",2)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
         <f>_xlfn.REGEXREPLACE(B3,"\{(.*?)\}|\*(.*?)\*","$1")</f>
         <v>The (quick brown) fox jumps over the lazy dog.</v>
@@ -1513,7 +1536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469A7F93-5D73-45B6-BB59-575C06EC4AA0}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1842,7 +1865,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView topLeftCell="E2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
I am getting closer to understanding the difference between option 1 and option 2
</commit_message>
<xml_diff>
--- a/CH-169 Extract From Text Part 2.xlsx
+++ b/CH-169 Extract From Text Part 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7557770D-0B60-4BE9-8D62-448AD1C808FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBD7597-35D1-4F50-8364-A4975F12434C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -61,18 +61,11 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="2">
+  <futureMetadata name="XLRICHVALUE" count="1">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
@@ -82,12 +75,9 @@
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="2">
+  <valueMetadata count="1">
     <bk>
       <rc t="2" v="0"/>
-    </bk>
-    <bk>
-      <rc t="2" v="1"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -870,16 +860,11 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
   <rv s="0">
     <fb t="e">#N/A</fb>
     <v>6</v>
     <v>7</v>
-  </rv>
-  <rv s="0">
-    <fb t="e">#N/A</fb>
-    <v>6</v>
-    <v>9</v>
   </rv>
 </rvData>
 </file>
@@ -1343,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B171B0C-5D2A-4231-8B3D-1BA0BFDBF0CC}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1467,51 +1452,33 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="e" cm="1" vm="1">
-        <f t="array" ref="B12">_xlfn.REGEXEXTRACT(B3,"(\{(.+?)\})|(\*(.+?)\*)",2)</f>
+        <f t="array" ref="B12">_xlfn.REGEXEXTRACT(B3,"(\{(.+?)\})|(\*(.*?)\*)", )</f>
         <v>#N/A</v>
       </c>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="e" cm="1" vm="1">
-        <f t="array" ref="B13">_xlfn.REGEXEXTRACT(B4,"(\{(.+?)\})|(\*(.+?)\*)",2)</f>
+        <f t="array" ref="B13">_xlfn.REGEXEXTRACT(B4,"(\{(.+?)\})|(\*(.*?)\*)", )</f>
         <v>#N/A</v>
       </c>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str" cm="1">
-        <f t="array" ref="B14:E14">_xlfn.REGEXEXTRACT(B5,"(\{(.+?)\})|(\*(.+?)\*)",2)</f>
+        <f t="array" ref="B14">_xlfn.REGEXEXTRACT(B5,"(\{(.+?)\})|(\*(.*?)\*)", )</f>
         <v>{beach for}</v>
-      </c>
-      <c r="C14" t="str">
-        <v>beach for</v>
-      </c>
-      <c r="D14" s="5" t="e" vm="2">
-        <v>#N/A</v>
-      </c>
-      <c r="E14" t="e" vm="2">
-        <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str" cm="1">
-        <f t="array" ref="B15:E15">_xlfn.REGEXEXTRACT(B6,"(\{(.+?)\})|(\*(.+?)\*)",2)</f>
+        <f t="array" ref="B15">_xlfn.REGEXEXTRACT(B6,"(\{(.+?)\})|(\*(.*?)\*)", )</f>
         <v>{rich}</v>
-      </c>
-      <c r="C15" t="str">
-        <v>rich</v>
-      </c>
-      <c r="D15" s="5" t="e" vm="2">
-        <v>#N/A</v>
-      </c>
-      <c r="E15" t="e" vm="2">
-        <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="e" cm="1" vm="1">
-        <f t="array" ref="B16">_xlfn.REGEXEXTRACT(B7,"(\{(.+?)\})|(\*(.+?)\*)",2)</f>
+        <f t="array" ref="B16">_xlfn.REGEXEXTRACT(B7,"(\{(.+?)\})|(\*(.*?)\*)", )</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1713,10 +1680,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83ADB577-E88F-434D-B48D-C1BDB2BB9EEB}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1852,6 +1819,48 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <v>playing guitar</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="str" cm="1">
+        <f t="array" ref="B17">_xlfn.REGEXEXTRACT(B3,"\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",1)</f>
+        <v>(quick brown)</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="str" cm="1">
+        <f t="array" ref="B18:C18">_xlfn.REGEXEXTRACT(B4,"\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",1)</f>
+        <v>[reading books]</v>
+      </c>
+      <c r="C18" t="str">
+        <v>[Walking]</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="str" cm="1">
+        <f t="array" ref="B19:C19">_xlfn.REGEXEXTRACT(B5,"\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",1)</f>
+        <v>{beach for}</v>
+      </c>
+      <c r="C19" t="str">
+        <v>*fun*</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="str" cm="1">
+        <f t="array" ref="B20:D20">_xlfn.REGEXEXTRACT(B6,"\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",1)</f>
+        <v>(chocolate cake)</v>
+      </c>
+      <c r="C20" t="str">
+        <v>(delicious)</v>
+      </c>
+      <c r="D20" s="5" t="str">
+        <v>{rich}</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="str" cm="1">
+        <f t="array" ref="B21">_xlfn.REGEXEXTRACT(B7,"\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",1)</f>
+        <v>[playing guitar]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I now understand where the NAs are coming from. Major step forward
</commit_message>
<xml_diff>
--- a/CH-169 Extract From Text Part 2.xlsx
+++ b/CH-169 Extract From Text Part 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBD7597-35D1-4F50-8364-A4975F12434C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5788F959-F58A-4AD2-AE88-C863105DDFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,11 +61,18 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="1">
+  <futureMetadata name="XLRICHVALUE" count="2">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
@@ -75,16 +82,19 @@
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="1">
+  <valueMetadata count="2">
     <bk>
       <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="26">
   <si>
     <t>Question</t>
   </si>
@@ -339,6 +349,12 @@
   </si>
   <si>
     <t>beach for</t>
+  </si>
+  <si>
+    <t>I now understand where the NA comes from.</t>
+  </si>
+  <si>
+    <t>This represents the first match from each capture group.</t>
   </si>
 </sst>
 </file>
@@ -860,11 +876,16 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
   <rv s="0">
     <fb t="e">#N/A</fb>
     <v>6</v>
     <v>7</v>
+  </rv>
+  <rv s="0">
+    <fb t="e">#N/A</fb>
+    <v>6</v>
+    <v>9</v>
   </rv>
 </rvData>
 </file>
@@ -1680,17 +1701,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83ADB577-E88F-434D-B48D-C1BDB2BB9EEB}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.09765625" customWidth="1"/>
     <col min="2" max="2" width="52.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.3984375" customWidth="1"/>
+    <col min="3" max="3" width="6.09765625" customWidth="1"/>
     <col min="4" max="4" width="24.69921875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1821,13 +1842,13 @@
         <v>playing guitar</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="str" cm="1">
         <f t="array" ref="B17">_xlfn.REGEXEXTRACT(B3,"\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",1)</f>
         <v>(quick brown)</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str" cm="1">
         <f t="array" ref="B18:C18">_xlfn.REGEXEXTRACT(B4,"\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",1)</f>
         <v>[reading books]</v>
@@ -1836,7 +1857,7 @@
         <v>[Walking]</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="str" cm="1">
         <f t="array" ref="B19:C19">_xlfn.REGEXEXTRACT(B5,"\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",1)</f>
         <v>{beach for}</v>
@@ -1845,7 +1866,7 @@
         <v>*fun*</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="str" cm="1">
         <f t="array" ref="B20:D20">_xlfn.REGEXEXTRACT(B6,"\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",1)</f>
         <v>(chocolate cake)</v>
@@ -1857,10 +1878,43 @@
         <v>{rich}</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="str" cm="1">
         <f t="array" ref="B21">_xlfn.REGEXEXTRACT(B7,"\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",1)</f>
         <v>[playing guitar]</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="e" cm="1" vm="2">
+        <f t="array" ref="B26:F26">_xlfn.REGEXEXTRACT(B24,"%(.*?)%|\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C26" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="D26" s="5" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="E26" t="str">
+        <v>beach for</v>
+      </c>
+      <c r="F26" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I think I understand what is going on.
</commit_message>
<xml_diff>
--- a/CH-169 Extract From Text Part 2.xlsx
+++ b/CH-169 Extract From Text Part 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5788F959-F58A-4AD2-AE88-C863105DDFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9677BC3-5167-4527-BEDB-CCB6E64D0AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="28">
   <si>
     <t>Question</t>
   </si>
@@ -356,6 +356,12 @@
   <si>
     <t>This represents the first match from each capture group.</t>
   </si>
+  <si>
+    <t>The (chocolate cake) was (delicious) and {rich}.</t>
+  </si>
+  <si>
+    <t>Okay, you can't use 2 because it just returns the first match.</t>
+  </si>
 </sst>
 </file>
 
@@ -827,6 +833,385 @@
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>23446</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>58614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>521677</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>52753</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EEBC055-D80C-165C-F974-2AF15AF87B1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4601308" y="1746737"/>
+          <a:ext cx="5720861" cy="8962293"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>In regex, conditional replacement strings allow you to insert text based on whether a specific capturing group exists and is not empty. Here are some common options for conditional replacement strings:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>1. **Basic Conditional Replacement**:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>   - Syntax: `${n:+text}`</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>   - Description: Inserts `text` if the `n`-th capturing group exists and is not empty.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>   - Example: `${2:+, }` inserts `, ` if the second capturing group exists and is not empty.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>2. **Conditional Replacement with Else**:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>   - Syntax: `${n:+text1:text2}`</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>   - Description: Inserts `text1` if the `n`-th capturing group exists and is not empty; otherwise, inserts `text2`.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>   - Example: `${2:+, :; }` inserts `, ` if the second capturing group exists and is not empty; otherwise, inserts `; `.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>3. **Conditional Replacement with Default Value**:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>   - Syntax: `${n:-text}`</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>   - Description: Inserts `text` if the `n`-th capturing group does not exist or is empty.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>   - Example: `${2:-default}` inserts `default` if the second capturing group does not exist or is empty.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>### Example in Python</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>Here's an example of how you can use these conditional replacement strings in Python:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>```python</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>import re</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>text = "12345"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>pattern = r'(\d{2})(\d{3})?'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>replacement = r'$1${2:+, }'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>result = re.sub(pattern, replacement, text)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>print(result)  # Output: 12, 345</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>text = "12"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>result = re.sub(pattern, replacement, text)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>print(result)  # Output: 12</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>```</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>In this example:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>- For the string `"12345"`, the second capturing group exists and is not empty, so `, ` is inserted.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>- For the string `"12"`, the second capturing group does not exist, so nothing is inserted.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>Feel free to experiment with these options and let me know if you have any questions or need further assistance!</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>58615</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>128954</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>603739</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>5862</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5A07553-A5F4-8265-969F-B23663E063FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4636477" y="10961077"/>
+          <a:ext cx="5767754" cy="2162908"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Sure! The replacement string ${6:+:, } uses a conditional replacement syntax in regex. This syntax allows you to insert text based on whether a specific capturing group exists and is not empty. Here's a breakdown of what it does and why it's constructed this way:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>${6:...}: This part of the syntax refers to the sixth capturing group in your regex pattern. The 6 indicates that the condition is based on the sixth capturing group.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>:+: This is the conditional operator. It means "if the capturing group exists and is not empty, then...".</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>:,: This is the text to be inserted if the condition is met. In this case, it will insert :,.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Putting it all together, ${6:+:, } means "if the sixth capturing group exists and is not empty, insert :,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1349,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B171B0C-5D2A-4231-8B3D-1BA0BFDBF0CC}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1524,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469A7F93-5D73-45B6-BB59-575C06EC4AA0}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1696,15 +2081,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83ADB577-E88F-434D-B48D-C1BDB2BB9EEB}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1915,6 +2301,136 @@
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="e" cm="1" vm="2">
+        <f t="array" ref="B37:F37">_xlfn.REGEXEXTRACT(B31,"%(.*?)%|\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C37" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="D37" s="5" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="E37" t="str">
+        <v>beach for</v>
+      </c>
+      <c r="F37" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="e" cm="1" vm="2">
+        <f t="array" ref="B38:F38">_xlfn.REGEXEXTRACT(B32,"%(.*?)%|\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C38" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="D38" s="5" t="str">
+        <v>reading books</v>
+      </c>
+      <c r="E38" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="F38" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="e" cm="1" vm="2">
+        <f t="array" ref="B39:F39">_xlfn.REGEXEXTRACT(B33,"%(.*?)%|\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C39" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="D39" s="5" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="E39" t="str">
+        <v>beach for</v>
+      </c>
+      <c r="F39" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="e" cm="1" vm="2">
+        <f t="array" ref="B40:F40">_xlfn.REGEXEXTRACT(B34,"%(.*?)%|\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C40" t="str">
+        <v>chocolate cake</v>
+      </c>
+      <c r="D40" s="5" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="E40" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="F40" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="e" cm="1" vm="2">
+        <f t="array" ref="B41:F41">_xlfn.REGEXEXTRACT(B35,"%(.*?)%|\((.*?)\)|\[(.*?)\]|\{(.*?)\}|\*(.*?)\*",2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C41" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="D41" s="5" t="str">
+        <v>playing guitar</v>
+      </c>
+      <c r="E41" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+      <c r="F41" t="e" vm="2">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>